<commit_message>
20210709 update from local
</commit_message>
<xml_diff>
--- a/data/20190611 - pilot metadata.xlsx
+++ b/data/20190611 - pilot metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettell/Documents/Repositories/pilot_paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12D1E6AB-C80F-D448-8518-3EE62C48E674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFEBB94-D011-3440-92C9-E9AE9D7188AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="680" windowWidth="20000" windowHeight="15580" xr2:uid="{830227E0-9704-ED41-949B-8B6EA93F7D52}"/>
+    <workbookView xWindow="1500" yWindow="500" windowWidth="26060" windowHeight="15580" xr2:uid="{830227E0-9704-ED41-949B-8B6EA93F7D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339BFAA8-2C5F-2047-AD51-2C36656222B8}">
   <dimension ref="B1:AS99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ8" sqref="AQ8:AQ94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7072,6 +7072,9 @@
       <c r="AK81" t="s">
         <v>68</v>
       </c>
+      <c r="AL81" t="s">
+        <v>158</v>
+      </c>
       <c r="AO81" t="s">
         <v>67</v>
       </c>
@@ -7080,6 +7083,9 @@
       </c>
       <c r="AQ81" t="s">
         <v>162</v>
+      </c>
+      <c r="AR81" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="2:44" x14ac:dyDescent="0.2">

</xml_diff>